<commit_message>
ready to execute 1
</commit_message>
<xml_diff>
--- a/target/test-classes/bookShelvesData.xlsx
+++ b/target/test-classes/bookShelvesData.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Model Name</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Mika Leatherette Study Chair In Scarlet Red Colour</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>5</v>

</xml_diff>